<commit_message>
Updated prices (ref year 2022, but introduced USGS source)
</commit_message>
<xml_diff>
--- a/data-raw/um.xlsx
+++ b/data-raw/um.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/clccr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="11_AD4D5CB4E552A5DACE1C64C0901D4AE65BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2229953-3AA8-412B-8D6D-1C6D2E84C98F}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="11_AD4D5CB4E552A5DACE1C64C0901D4AE65BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A9B5E88-6EAA-4107-AB20-8817349AEFD1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="imf" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="85">
   <si>
     <t>legend</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>kwh</t>
+  </si>
+  <si>
+    <t>carat</t>
+  </si>
+  <si>
+    <t>short t</t>
   </si>
 </sst>
 </file>
@@ -912,10 +918,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900FD9F8-92C3-463F-81FD-F9E405544B04}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,6 +1034,28 @@
       </c>
       <c r="C10">
         <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12">
+        <v>907.18499999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>